<commit_message>
Added Joins and Update, Delete, and Alter Table
</commit_message>
<xml_diff>
--- a/sql/G2T.xlsx
+++ b/sql/G2T.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nnesb\Documents\Programs\Okanagan College\Class Code\G2T-Class-Code\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F77227-4748-45E2-A953-D248948F2303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C019B849-7F7A-43D2-90E8-D7DB217F3CB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8A524C9F-988B-43AF-8EA1-5B32B97CCC5B}"/>
   </bookViews>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF01AAF9-3237-494B-BB96-BA2EC704F4BB}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,8 +491,8 @@
         <v>3</v>
       </c>
       <c r="C2" s="3">
-        <f>10^10</f>
-        <v>10000000000</v>
+        <f>10^9</f>
+        <v>1000000000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,6 +560,9 @@
       <c r="C8" s="3">
         <v>1000000000</v>
       </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -571,9 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2150CB1D-88CB-437E-A675-4B0209761103}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Basic Code for MySQL using Node
</commit_message>
<xml_diff>
--- a/sql/G2T.xlsx
+++ b/sql/G2T.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nnesb\Documents\Programs\Okanagan College\Class Code\G2T-Class-Code\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C019B849-7F7A-43D2-90E8-D7DB217F3CB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69EF685-28E3-4E63-8404-A2A2B7F99570}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8A524C9F-988B-43AF-8EA1-5B32B97CCC5B}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2150CB1D-88CB-437E-A675-4B0209761103}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>